<commit_message>
siste endring jævla møkkadag
</commit_message>
<xml_diff>
--- a/barnehage/kgdata.xlsx
+++ b/barnehage/kgdata.xlsx
@@ -971,7 +971,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1046,121 +1046,73 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
-      </c>
-      <c r="C2" t="n">
-        <v>11</v>
-      </c>
-      <c r="D2" t="n">
-        <v>12</v>
-      </c>
-      <c r="E2" t="n">
-        <v>6</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>ABC Kindergarten</t>
-        </is>
-      </c>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>2024-10-31</t>
-        </is>
-      </c>
-      <c r="M2" t="n">
-        <v>2000000</v>
-      </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
-      </c>
-      <c r="C3" t="n">
-        <v>9</v>
-      </c>
-      <c r="D3" t="n">
-        <v>10</v>
-      </c>
-      <c r="E3" t="n">
-        <v>5</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Sunshine Preschool	</t>
-        </is>
-      </c>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>2024-10-29</t>
-        </is>
-      </c>
-      <c r="M3" t="n">
-        <v>10</v>
-      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
-      </c>
-      <c r="C4" t="n">
         <v>7</v>
       </c>
-      <c r="D4" t="n">
-        <v>8</v>
-      </c>
-      <c r="E4" t="n">
-        <v>4</v>
-      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>ABC Kindergarten</t>
-        </is>
-      </c>
+      <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>2024-10-29</t>
-        </is>
-      </c>
-      <c r="M4" t="n">
-        <v>300200</v>
-      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D5" t="n">
+        <v>12</v>
+      </c>
+      <c r="E5" t="n">
         <v>6</v>
-      </c>
-      <c r="E5" t="n">
-        <v>3</v>
       </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
@@ -1174,11 +1126,11 @@
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-10-31</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>10000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="6">
@@ -1186,16 +1138,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
@@ -1203,7 +1155,7 @@
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr">
         <is>
-          <t>ABC Kindergarten</t>
+          <t xml:space="preserve">Sunshine Preschool	</t>
         </is>
       </c>
       <c r="K6" t="inlineStr"/>
@@ -1213,7 +1165,7 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>20000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -1221,25 +1173,130 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>ABC Kindergarten</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>2024-10-29</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
+        <v>300200</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" t="n">
+        <v>6</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3</v>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>ABC Kindergarten</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>2024-10-29</t>
+        </is>
+      </c>
+      <c r="M8" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>ABC Kindergarten</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>2024-10-29</t>
+        </is>
+      </c>
+      <c r="M9" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>